<commit_message>
Update project with new features
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin/NewFolder/maven/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549499D8-58B9-EB42-9E4B-B971491AA3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42B788E-EF7B-E341-96CB-04D9ADC1AEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1540" yWindow="2840" windowWidth="25600" windowHeight="13880" xr2:uid="{F97F2164-B85F-614B-89FC-F5A84FDE747C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="103">
   <si>
     <t>id</t>
   </si>
@@ -60,59 +60,299 @@
     <t>homePageUrl</t>
   </si>
   <si>
-    <t>http://cargill.planbox.com/default/Login?signInWithSecretKey=true</t>
-  </si>
-  <si>
-    <t>http://cargill.planbox.com/default/challenges</t>
-  </si>
-  <si>
-    <t>http://cargill.planbox.com/default/ideas</t>
-  </si>
-  <si>
-    <t>http://cargill.planbox.com/default/home/homepage</t>
-  </si>
-  <si>
-    <t>https://dow.planbox.com/default/challenges</t>
-  </si>
-  <si>
-    <t>http://dow.planbox.com/default/Login?signInWithSecretKey=true</t>
-  </si>
-  <si>
-    <t>http://dow.planbox.com/default/ideas</t>
-  </si>
-  <si>
-    <t>http://dow.planbox.com/default/home/homepage</t>
-  </si>
-  <si>
-    <t>https://galp.planbox.com/default/Login?signInWithSecretKey=true</t>
-  </si>
-  <si>
-    <t>https://galp.planbox.com/default/challenges</t>
-  </si>
-  <si>
-    <t>https://galp.planbox.com/default/ideas</t>
-  </si>
-  <si>
-    <t>https://galp.planbox.com/default/home/homepage</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
-    <t>Cargil</t>
-  </si>
-  <si>
-    <t>Dow</t>
-  </si>
-  <si>
-    <t>Galp</t>
+    <t>https://iconplc.planbox.com/default/login?signinwithsecretkey=true</t>
+  </si>
+  <si>
+    <t>https://iconplc.planbox.com/default/challenges</t>
+  </si>
+  <si>
+    <t>https://iconplc.planbox.com/default/ideas</t>
+  </si>
+  <si>
+    <t>https://iconplc.planbox.com/default/Home/HomePage</t>
+  </si>
+  <si>
+    <t>iconplc</t>
+  </si>
+  <si>
+    <t>https://libertymutual.planbox.com/default/Login?signInWithSecretKey=true</t>
+  </si>
+  <si>
+    <t>https://libertymutual.planbox.com/default/ideas</t>
+  </si>
+  <si>
+    <t>https://libertymutual.planbox.com/default/Home/Homepage</t>
+  </si>
+  <si>
+    <t>libertymutual</t>
+  </si>
+  <si>
+    <t>https://libertymutual.planbox.com/default/challenges</t>
+  </si>
+  <si>
+    <t>https://scouting.planbox.com/default/Login?signinwithsecretkey=true</t>
+  </si>
+  <si>
+    <t>https://scouting.planbox.com/default/challenges</t>
+  </si>
+  <si>
+    <t>https://scouting.planbox.com/default/ideas</t>
+  </si>
+  <si>
+    <t>https://scouting.planbox.com/default/home/homepage</t>
+  </si>
+  <si>
+    <t>Scouting</t>
+  </si>
+  <si>
+    <t>a2c7259521324fc9a15273867531b27f:MojOdmjaPZg2f7w8Au4xxNJ2aIleEpmFxZ6vCeve7eS5oNOvIhO7IefQ6ly7wuD7m311HbDyr4jGEQCATziPdWlN7axU0ykWb5prqExWHpX8TNAfMkucj2cwACEuZqcE</t>
+  </si>
+  <si>
+    <t>https://imagine.planbox.com/default//Login?signinwithsecretkey=true</t>
+  </si>
+  <si>
+    <t>https://imagine.planbox.com/default/challenges</t>
+  </si>
+  <si>
+    <t>https://imagine.planbox.com/default/ideas</t>
+  </si>
+  <si>
+    <t>https://imagine.planbox.com/default/home/homepage</t>
+  </si>
+  <si>
+    <t>Imagine</t>
+  </si>
+  <si>
+    <t>https://statefarm.planbox.com/default//Login?signinwithsecretkey=true</t>
+  </si>
+  <si>
+    <t>https://statefarm.planbox.com/default/challenges</t>
+  </si>
+  <si>
+    <t>https://statefarm.planbox.com/default/ideas</t>
+  </si>
+  <si>
+    <t>Statefarm</t>
+  </si>
+  <si>
+    <t>https://statefarm.planbox.com/default/home/homepage</t>
+  </si>
+  <si>
+    <t>https://bio-rad.planbox.com/default/Login?signinwithsecretkey=true</t>
+  </si>
+  <si>
+    <t>https://bio-rad.planbox.com/default/Challenges</t>
+  </si>
+  <si>
+    <t>https://bio-rad.planbox.com/default/ideas</t>
+  </si>
+  <si>
+    <t>bio-rad</t>
+  </si>
+  <si>
+    <t>https://bio-rad.planbox.com/default/home/homepage</t>
+  </si>
+  <si>
+    <t>https://curi.planbox.com/default//Login?signinwithsecretkey=true</t>
+  </si>
+  <si>
+    <t>https://curi.planbox.com/default/challenges</t>
+  </si>
+  <si>
+    <t>https://curi.planbox.com/default/ideas</t>
+  </si>
+  <si>
+    <t>https://curi.planbox.com/default/home/homepage</t>
+  </si>
+  <si>
+    <t>Curi</t>
+  </si>
+  <si>
+    <t>https://shaw.planbox.com/default//Login?signinwithsecretkey=true</t>
+  </si>
+  <si>
+    <t>https://shaw.planbox.com/default/challenges</t>
+  </si>
+  <si>
+    <t>https://shaw.planbox.com/default/ideas</t>
+  </si>
+  <si>
+    <t>https://shaw.planbox.com/default/home/homepage</t>
+  </si>
+  <si>
+    <t>Shaw</t>
+  </si>
+  <si>
+    <t>https://stobg.planbox.com/default/Login?signinwithsecretkey=true</t>
+  </si>
+  <si>
+    <t>https://stobg.planbox.com/default/challenges</t>
+  </si>
+  <si>
+    <t>https://stobg.planbox.com/default/ideas</t>
+  </si>
+  <si>
+    <t>https://stobg.planbox.com/default/home/homepage</t>
+  </si>
+  <si>
+    <t>Stobg</t>
+  </si>
+  <si>
+    <t>https://idearally.planbox.com/default/Login?signInWithSecretKey=true</t>
+  </si>
+  <si>
+    <t>https://idearally.planbox.com/default/challenges</t>
+  </si>
+  <si>
+    <t>https://idearally.planbox.com/default/ideas</t>
+  </si>
+  <si>
+    <t>https://idearally.planbox.com/default/home/homepage</t>
+  </si>
+  <si>
+    <t>Idearally</t>
+  </si>
+  <si>
+    <t>https://bakertilly-sandbox.planbox.com/default/Login?signInWithSecretKey=true</t>
+  </si>
+  <si>
+    <t>https://bakertilly-sandbox.planbox.com/default/challenges</t>
+  </si>
+  <si>
+    <t>https://bakertilly-sandbox.planbox.com/default/ideas</t>
+  </si>
+  <si>
+    <t>https://bakertilly-sandbox.planbox.com/default/home/homepage</t>
+  </si>
+  <si>
+    <t>Bakertilly</t>
+  </si>
+  <si>
+    <t>Web2</t>
+  </si>
+  <si>
+    <t>Web3</t>
+  </si>
+  <si>
+    <t>https://innovate.hollister.com/default/login?signinwithsecretkey=true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://innovate.hollister.com/default/challenges </t>
+  </si>
+  <si>
+    <t>https://innovate.hollister.com/default/ideas</t>
+  </si>
+  <si>
+    <t>https://innovate.hollister.com/default/home/homepage</t>
+  </si>
+  <si>
+    <t>Innovate.hollister</t>
+  </si>
+  <si>
+    <t>d790fc53d2424e3e800be26b1181620d:XhmnoBbZWNuVByDK34XgxV64syPE8um1vPD3xk5DW0Iz6K37CwS3zBMUSjLGnbxWfBI1NNGamiDyYiSTR8yUN1oQSP0aX7GvOAPcLxjZHkMsqcX6HiBte4icmIGBm4Ib</t>
+  </si>
+  <si>
+    <t>https://kearney.planbox.com/default/Login?signinwithsecretkey=true</t>
+  </si>
+  <si>
+    <t>https://kearney.planbox.com/default/challenges</t>
+  </si>
+  <si>
+    <t>https://kearney.planbox.com/default/ideas</t>
+  </si>
+  <si>
+    <t>https://kearney.planbox.com/default/home/homepage</t>
+  </si>
+  <si>
+    <t>Kearney</t>
+  </si>
+  <si>
+    <t>https://launchpad2.planbox.com/default/Login?signInWithSecretKey=true</t>
+  </si>
+  <si>
+    <t>https://launchpad2.planbox.com/default/challenges</t>
+  </si>
+  <si>
+    <t>https://launchpad2.planbox.com/default/ideas</t>
+  </si>
+  <si>
+    <t>https://launchpad2.planbox.com/default/home/homepage</t>
+  </si>
+  <si>
+    <t>Launchpad2</t>
+  </si>
+  <si>
+    <t>https://techforgood.planbox.com/default//Login?signinwithsecretkey=true</t>
+  </si>
+  <si>
+    <t>https://techforgood.planbox.com/default/challenges</t>
+  </si>
+  <si>
+    <t>https://techforgood.planbox.com/default/ideas</t>
+  </si>
+  <si>
+    <t>https://techforgood.planbox.com/default/home/homepage</t>
+  </si>
+  <si>
+    <t>Techforgood</t>
+  </si>
+  <si>
+    <t>https://verizon.planbox.com/default/Login?signinwithsecretkey=true</t>
+  </si>
+  <si>
+    <t>https://verizon.planbox.com/default/challenges</t>
+  </si>
+  <si>
+    <t>https://verizon.planbox.com/default/ideas</t>
+  </si>
+  <si>
+    <t>https://verizon.planbox.com/default/home/homepage</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>https://appliedsystems.planbox.com/default/Login?signInWithSecretKey=true</t>
+  </si>
+  <si>
+    <t>https://appliedsystems.planbox.com/default/ideas</t>
+  </si>
+  <si>
+    <t>https://appliedsystems.planbox.com/default/home/homepage</t>
+  </si>
+  <si>
+    <t>Appliedsystems</t>
+  </si>
+  <si>
+    <t>https://appliedsystems.planbox.com/default/challenges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">web4 </t>
+  </si>
+  <si>
+    <t>https://innovationstation.planbox.com/default//Login?signinwithsecretkey=true</t>
+  </si>
+  <si>
+    <t>https://innovationstation.planbox.com/default/ideas</t>
+  </si>
+  <si>
+    <t>https://innovationstation.planbox.com/default/home/homepage</t>
+  </si>
+  <si>
+    <t>Innovationstation</t>
+  </si>
+  <si>
+    <t>https://innovationstation.planbox.com/default/challenges</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,26 +367,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -170,11 +390,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -491,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FCDA1F-0D51-C045-9FB9-22859F94D090}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -507,7 +724,7 @@
     <col min="7" max="7" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,85 +744,35 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{95105C6E-A200-3046-94EE-65DB90734152}"/>
-    <hyperlink ref="E3:F3" r:id="rId2" display="https://dow.planbox.com/default/challenges" xr:uid="{4BD15BAE-D9E3-5646-8C40-9FD9A61E7C89}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{E851C3BC-5ADD-9644-9193-24D81A4E2FC9}"/>
-    <hyperlink ref="F3" r:id="rId4" xr:uid="{24656144-6499-124F-AE58-C1C69BDC27ED}"/>
-    <hyperlink ref="B3" r:id="rId5" xr:uid="{AE9332C8-6DD2-7E48-9940-6793B7652DCA}"/>
-    <hyperlink ref="F2" r:id="rId6" xr:uid="{C1A599A3-9592-2D49-AFE0-965A92C3E4EB}"/>
-    <hyperlink ref="E2" r:id="rId7" xr:uid="{C5EAC9DB-F50C-3E4D-85AF-8DBDCE84AA02}"/>
-    <hyperlink ref="D2" r:id="rId8" xr:uid="{69A94CE0-20B1-0A48-AE1E-103556B8EDB8}"/>
-    <hyperlink ref="B2" r:id="rId9" xr:uid="{13824654-8B83-1A4E-9270-B97231396217}"/>
-    <hyperlink ref="B4" r:id="rId10" xr:uid="{C626A997-4E3F-6F41-A28A-21AB269D073F}"/>
-    <hyperlink ref="E4:F4" r:id="rId11" display="https://galp.planbox.com/default/challenges" xr:uid="{FF0A053B-0BC2-E847-930A-F6866E7A8F3A}"/>
-    <hyperlink ref="E4" r:id="rId12" xr:uid="{567C677F-8F50-BE49-A171-0549512C3FE1}"/>
-    <hyperlink ref="F4" r:id="rId13" xr:uid="{19ACD4BF-B256-9249-AC46-E2D66FC48449}"/>
-    <hyperlink ref="D4" r:id="rId14" xr:uid="{42B32DDE-87F3-6941-ACED-EC95D1216A11}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{EBBB433C-20FF-1E4A-A663-53539D1FE271}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{EEF04FD6-65CB-A748-A499-1D4111418D37}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{592FFC33-630C-A64C-9E4F-75E343034E59}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{87F7A376-DCD1-D34E-9B57-9C56D75F28A3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -613,14 +780,469 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB2DA10-CE78-3E4B-B22D-00701690B968}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="145.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{CA2D8694-7C9F-8045-8371-FAF91CE87B86}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{35ABEF39-6BAB-5440-82CD-E56B489BA546}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{725FB047-0B77-254F-84BD-2BF4A7D7F491}"/>
+    <hyperlink ref="F3" r:id="rId4" xr:uid="{899FDD02-FD61-7241-B69E-00FF9E861BEC}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{63DAB723-22E3-8946-8A7E-9CF7B5833F3F}"/>
+    <hyperlink ref="D2" r:id="rId6" xr:uid="{C7AE4256-70B5-8B49-A346-2740E36A563F}"/>
+    <hyperlink ref="F2" r:id="rId7" xr:uid="{FCB4F05C-3168-8F41-9C3D-9829961C60D2}"/>
+    <hyperlink ref="E2" r:id="rId8" xr:uid="{E323F6F8-480C-1B40-9AC1-25C2AB8A604A}"/>
+    <hyperlink ref="D1" r:id="rId9" xr:uid="{76569C92-DCC8-E746-B8B4-A669D379261F}"/>
+    <hyperlink ref="B1" r:id="rId10" xr:uid="{726EFAF0-96F0-8146-8343-C399A5212A8E}"/>
+    <hyperlink ref="F1" r:id="rId11" xr:uid="{52553E17-F525-6B44-9DDF-6697B906B7AC}"/>
+    <hyperlink ref="E1" r:id="rId12" xr:uid="{812F4A77-1F88-0142-BCF9-44FDA2A62F7A}"/>
+    <hyperlink ref="B6" r:id="rId13" xr:uid="{7A21335A-07E6-FA4F-93D9-82F2BE1D7834}"/>
+    <hyperlink ref="D6" r:id="rId14" xr:uid="{B08F3C3F-CC03-2543-BDCE-D803873BCDF7}"/>
+    <hyperlink ref="E6" r:id="rId15" xr:uid="{63074FD9-F13F-D343-8401-AB6F2AC05E3F}"/>
+    <hyperlink ref="F6" r:id="rId16" xr:uid="{BCF39189-0B3C-404B-896A-7D2B2115110D}"/>
+    <hyperlink ref="B7" r:id="rId17" xr:uid="{72DC4105-64EF-9646-B002-41D37E684E0D}"/>
+    <hyperlink ref="D7" r:id="rId18" xr:uid="{DF555C3A-D502-544C-92D1-F0295FE38FCC}"/>
+    <hyperlink ref="E7" r:id="rId19" xr:uid="{196C354D-EF47-5B4A-8A19-CE5B858275E8}"/>
+    <hyperlink ref="F7" r:id="rId20" xr:uid="{9390B624-3CD7-2A49-8C75-CA83B6416F05}"/>
+    <hyperlink ref="B8" r:id="rId21" xr:uid="{411AC1A5-F9F4-8748-A648-4468A15D5C58}"/>
+    <hyperlink ref="D8" r:id="rId22" xr:uid="{EBE54AA1-E5C2-F640-A059-90CCD0C3CABB}"/>
+    <hyperlink ref="E8" r:id="rId23" xr:uid="{3674627F-39A9-8E48-8F96-F2772162DBCF}"/>
+    <hyperlink ref="F8" r:id="rId24" xr:uid="{87DA96B1-B2EA-CB46-9112-6DB712A08EBD}"/>
+    <hyperlink ref="B9" r:id="rId25" xr:uid="{459F1266-C3AB-C843-BF1E-D0A18C1F698D}"/>
+    <hyperlink ref="D9" r:id="rId26" xr:uid="{8A6394E7-2C3E-EF4A-AF0B-5D0CD0780E45}"/>
+    <hyperlink ref="E9" r:id="rId27" xr:uid="{BD4C7214-DB76-A24A-B0A9-647AA1D8F5AA}"/>
+    <hyperlink ref="F9" r:id="rId28" xr:uid="{68454F82-0F21-614E-B22D-963FE088A184}"/>
+    <hyperlink ref="B10" r:id="rId29" xr:uid="{7FD91B6C-DB99-694C-B556-0897BD0D9555}"/>
+    <hyperlink ref="D10" r:id="rId30" xr:uid="{5F41E132-AE0F-F54C-BE50-901E8674B844}"/>
+    <hyperlink ref="E10" r:id="rId31" xr:uid="{6CDE7991-7CA2-F541-A1D6-E325EF8756A1}"/>
+    <hyperlink ref="F10" r:id="rId32" xr:uid="{AD102D33-C62E-5C47-9625-E2C480EBDA84}"/>
+    <hyperlink ref="B11" r:id="rId33" xr:uid="{F5C87AC2-456E-7C41-BCAC-F0341E50C7DC}"/>
+    <hyperlink ref="D11" r:id="rId34" xr:uid="{29638548-E0BC-F44B-8A3C-61CEC4CBB7B3}"/>
+    <hyperlink ref="E11" r:id="rId35" xr:uid="{D2E2656E-17BD-0745-8F46-A6A611CB4FA1}"/>
+    <hyperlink ref="F11" r:id="rId36" xr:uid="{A690AA93-310E-3345-AD65-91E1D43ABCCB}"/>
+    <hyperlink ref="B12" r:id="rId37" xr:uid="{1E4B2E41-64C5-DA42-9F46-E6EC5A53B8DC}"/>
+    <hyperlink ref="D12" r:id="rId38" xr:uid="{B4013258-FF3B-6944-8B7A-BACB13F35224}"/>
+    <hyperlink ref="E12" r:id="rId39" xr:uid="{AD39E25C-7354-7545-81C5-239948248A4D}"/>
+    <hyperlink ref="F12" r:id="rId40" xr:uid="{E56C0763-3211-DC47-BAC2-6C4F5F16821C}"/>
+    <hyperlink ref="B16" r:id="rId41" xr:uid="{13557987-E308-FA4E-9BFB-2D0ECA44DF3B}"/>
+    <hyperlink ref="D16" r:id="rId42" xr:uid="{EC02017C-4CCE-AD4A-8B87-AC121CA9D5E4}"/>
+    <hyperlink ref="E16" r:id="rId43" xr:uid="{5EFE9077-E08F-2C4B-A820-898C075F4107}"/>
+    <hyperlink ref="F16" r:id="rId44" xr:uid="{ECE0BBAB-6F8A-3547-8362-9E792A7F7589}"/>
+    <hyperlink ref="C16" r:id="rId45" display="https://bakertilly-sandbox.planbox.com/default/Login?signInWithSecretKey=true" xr:uid="{77F19050-4599-5144-B984-1189D97D10B1}"/>
+    <hyperlink ref="B17" r:id="rId46" xr:uid="{B59A3678-BAF1-A245-8A2B-B32E1EB22A49}"/>
+    <hyperlink ref="D17" r:id="rId47" xr:uid="{1B3B58CC-52C3-A749-99F4-E7EA1A3E8628}"/>
+    <hyperlink ref="E17" r:id="rId48" xr:uid="{49F5616C-E36F-8E47-9952-BA6F7CEE5B9B}"/>
+    <hyperlink ref="F17" r:id="rId49" xr:uid="{88A348DF-4C72-3C4A-BA5E-6266CABCF1E5}"/>
+    <hyperlink ref="B18" r:id="rId50" xr:uid="{BF4AE47F-71A0-394C-BAC8-30131F73949C}"/>
+    <hyperlink ref="D18" r:id="rId51" xr:uid="{D85AD82C-4EAF-0445-A6FC-1F4364F106F5}"/>
+    <hyperlink ref="E18" r:id="rId52" xr:uid="{AA9872D9-987E-2E46-A6C4-80E5095F4096}"/>
+    <hyperlink ref="F18" r:id="rId53" xr:uid="{A9BEC471-5052-8B4B-8C8F-9A093D6D6820}"/>
+    <hyperlink ref="B19" r:id="rId54" xr:uid="{2DCEC506-C831-F44A-B0D4-164BA3C9A1AD}"/>
+    <hyperlink ref="D19" r:id="rId55" xr:uid="{2318A444-3D0E-2545-9A2A-F89E120392C5}"/>
+    <hyperlink ref="E19" r:id="rId56" xr:uid="{79F9EBF9-4D4D-364A-B1C2-479B5CAAB4D7}"/>
+    <hyperlink ref="F19" r:id="rId57" xr:uid="{B032435F-9885-B949-8FEE-EA95DEB1077A}"/>
+    <hyperlink ref="B20" r:id="rId58" xr:uid="{1CF48759-75FB-A442-AE90-1A4E2F76E39B}"/>
+    <hyperlink ref="D20" r:id="rId59" xr:uid="{2B6E8504-394C-5944-9B7D-3280DF0D9F16}"/>
+    <hyperlink ref="E20" r:id="rId60" xr:uid="{AAF90295-9CB1-6543-BDDD-A4C83D250791}"/>
+    <hyperlink ref="F20" r:id="rId61" xr:uid="{BEF5433D-8817-CF48-B479-8D53A74488B0}"/>
+    <hyperlink ref="B21" r:id="rId62" xr:uid="{86526910-8198-C94A-8048-BD7BED9F7F81}"/>
+    <hyperlink ref="D21" r:id="rId63" xr:uid="{CF6378C0-2F62-774E-800E-2FFE49CD6347}"/>
+    <hyperlink ref="E21" r:id="rId64" xr:uid="{D6F50C62-501E-A04D-B977-7393BEA6B37B}"/>
+    <hyperlink ref="F21" r:id="rId65" xr:uid="{FE56074A-8F3A-524C-8CBB-209487607513}"/>
+    <hyperlink ref="B22" r:id="rId66" xr:uid="{F4F8CD0E-1036-8944-BAA5-ECF0D304D9ED}"/>
+    <hyperlink ref="D22" r:id="rId67" xr:uid="{A6DB1405-FBC5-254F-AE8C-213D29A73F96}"/>
+    <hyperlink ref="E22" r:id="rId68" xr:uid="{297B7EF0-F8F1-6949-B8EB-4813D1471F91}"/>
+    <hyperlink ref="F22" r:id="rId69" xr:uid="{412BD79C-0808-B440-A2D2-9D43A988D20F}"/>
+    <hyperlink ref="B25" r:id="rId70" xr:uid="{2ED45B5B-D639-2C43-9EF6-B46D64AAF109}"/>
+    <hyperlink ref="D25" r:id="rId71" xr:uid="{E860BC24-2E85-0040-B518-496C17A0A88C}"/>
+    <hyperlink ref="E25" r:id="rId72" xr:uid="{6F02C658-747D-9C4F-B16B-AC53F26AA9EE}"/>
+    <hyperlink ref="F25" r:id="rId73" xr:uid="{EA0A994F-F29C-FC49-B415-F1B8607A25DC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated example.txt with new content
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin/NewFolder/maven/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42B788E-EF7B-E341-96CB-04D9ADC1AEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093BEF53-552C-924E-BC38-28EB6FFBCF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1540" yWindow="2840" windowWidth="25600" windowHeight="13880" xr2:uid="{F97F2164-B85F-614B-89FC-F5A84FDE747C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="104">
   <si>
     <t>id</t>
   </si>
@@ -346,6 +346,9 @@
   </si>
   <si>
     <t>https://innovationstation.planbox.com/default/challenges</t>
+  </si>
+  <si>
+    <t>https://imagine.planbox.com/default//Login?signinwithsecretkey=true111</t>
   </si>
 </sst>
 </file>
@@ -708,7 +711,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FCDA1F-0D51-C045-9FB9-22859F94D090}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -767,12 +770,36 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{EBBB433C-20FF-1E4A-A663-53539D1FE271}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{EEF04FD6-65CB-A748-A499-1D4111418D37}"/>
     <hyperlink ref="F2" r:id="rId3" xr:uid="{592FFC33-630C-A64C-9E4F-75E343034E59}"/>
     <hyperlink ref="E2" r:id="rId4" xr:uid="{87F7A376-DCD1-D34E-9B57-9C56D75F28A3}"/>
+    <hyperlink ref="B3" r:id="rId5" xr:uid="{DD7C665D-411D-9C42-97E8-E4D70DEB56E4}"/>
+    <hyperlink ref="D3" r:id="rId6" xr:uid="{F28FA937-54E8-154F-9FD0-491A1E5BBD93}"/>
+    <hyperlink ref="E3" r:id="rId7" xr:uid="{45D23699-B4B5-744B-AB82-0E35EDB95B6A}"/>
+    <hyperlink ref="F3" r:id="rId8" xr:uid="{78E696E3-CA53-F647-8819-0B8369AE0173}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -783,7 +810,7 @@
   <dimension ref="B1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>